<commit_message>
Usano JSZIP para armar zip en la descarga
</commit_message>
<xml_diff>
--- a/produccion/plantillavacia.xlsx
+++ b/produccion/plantillavacia.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franco\Desktop\Programacion\proyectito\GeneradorCertificadosAATVAC\produccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Larroca\Desktop\Giuliano\ProyectoAATVAC\produccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8D1CE2-4ED7-4612-985E-40850D7A78C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{058E0D31-0E9D-44D5-B092-455ADA2A1B5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -60,13 +59,16 @@
   </si>
   <si>
     <t>Segundo Cargo</t>
+  </si>
+  <si>
+    <t>Apellido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,48 +435,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9363108F-4471-4CFF-9BDE-43ED2EAC786C}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="55.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="28.75" customWidth="1"/>
+    <col min="9" max="9" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reformas borniquisimas, se sacaron las firmas de TODOS LOS CERTIFICADOS del lado del codigo
</commit_message>
<xml_diff>
--- a/produccion/plantillavacia.xlsx
+++ b/produccion/plantillavacia.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
@@ -52,13 +52,7 @@
     <t>Fecha Emision</t>
   </si>
   <si>
-    <t>Direccion</t>
-  </si>
-  <si>
     <t>Centro de formacion</t>
-  </si>
-  <si>
-    <t>Segundo Cargo</t>
   </si>
   <si>
     <t>Apellido</t>
@@ -436,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -455,7 +449,7 @@
     <col min="9" max="9" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -463,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -477,14 +471,10 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="H1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>